<commit_message>
update timegpt and lag-llama
</commit_message>
<xml_diff>
--- a/Experiment_results/xlsx_format/ex_TimeGPT_and_Lag-Llama.xlsx
+++ b/Experiment_results/xlsx_format/ex_TimeGPT_and_Lag-Llama.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\ДИПЛОМНЫЙ проект\результаты экспериментов\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6427DDE6-89BE-4C6E-AF6C-39311A4FFB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81720003-5E40-4A91-A816-4695EFD1F6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист2" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="176">
   <si>
     <t>ETTh1</t>
   </si>
@@ -66,36 +66,6 @@
     <t>MSE</t>
   </si>
   <si>
-    <t>0.576</t>
-  </si>
-  <si>
-    <t>0.894</t>
-  </si>
-  <si>
-    <t>0.89</t>
-  </si>
-  <si>
-    <t>1.124</t>
-  </si>
-  <si>
-    <t>1.328</t>
-  </si>
-  <si>
-    <t>2.471</t>
-  </si>
-  <si>
-    <t>2.687</t>
-  </si>
-  <si>
-    <t>3.292</t>
-  </si>
-  <si>
-    <t>5.392</t>
-  </si>
-  <si>
-    <t>9.238</t>
-  </si>
-  <si>
     <t>0.435</t>
   </si>
   <si>
@@ -129,48 +99,6 @@
     <t>0.224</t>
   </si>
   <si>
-    <t>0.247</t>
-  </si>
-  <si>
-    <t>0.253</t>
-  </si>
-  <si>
-    <t>0.263</t>
-  </si>
-  <si>
-    <t>0.303</t>
-  </si>
-  <si>
-    <t>0.522</t>
-  </si>
-  <si>
-    <t>1.357</t>
-  </si>
-  <si>
-    <t>1.219</t>
-  </si>
-  <si>
-    <t>2.262</t>
-  </si>
-  <si>
-    <t>2.941</t>
-  </si>
-  <si>
-    <t>9.472</t>
-  </si>
-  <si>
-    <t>11.382</t>
-  </si>
-  <si>
-    <t>16.066</t>
-  </si>
-  <si>
-    <t>44.45</t>
-  </si>
-  <si>
-    <t>114.86</t>
-  </si>
-  <si>
     <t>0.254</t>
   </si>
   <si>
@@ -195,27 +123,9 @@
     <t>19.585</t>
   </si>
   <si>
-    <t>0.059</t>
-  </si>
-  <si>
-    <t>0.061</t>
-  </si>
-  <si>
-    <t>0.064</t>
-  </si>
-  <si>
-    <t>0.094</t>
-  </si>
-  <si>
     <t>7.53</t>
   </si>
   <si>
-    <t>0.013</t>
-  </si>
-  <si>
-    <t>0.035</t>
-  </si>
-  <si>
     <t>benchmark</t>
   </si>
   <si>
@@ -294,36 +204,6 @@
     <t>0.011</t>
   </si>
   <si>
-    <t>7.942</t>
-  </si>
-  <si>
-    <t>7.510</t>
-  </si>
-  <si>
-    <t>6.104</t>
-  </si>
-  <si>
-    <t>6.233</t>
-  </si>
-  <si>
-    <t>6.411</t>
-  </si>
-  <si>
-    <t>93.442</t>
-  </si>
-  <si>
-    <t>92.097</t>
-  </si>
-  <si>
-    <t>60.032</t>
-  </si>
-  <si>
-    <t>61.101</t>
-  </si>
-  <si>
-    <t>63.333</t>
-  </si>
-  <si>
     <t>1.667</t>
   </si>
   <si>
@@ -345,24 +225,9 @@
     <t>4.188</t>
   </si>
   <si>
-    <t>7.166</t>
-  </si>
-  <si>
     <t>2.459</t>
   </si>
   <si>
-    <t>2.676</t>
-  </si>
-  <si>
-    <t>5.452</t>
-  </si>
-  <si>
-    <t>3.320</t>
-  </si>
-  <si>
-    <t>9.295</t>
-  </si>
-  <si>
     <t>0.504</t>
   </si>
   <si>
@@ -378,9 +243,6 @@
     <t>0.965</t>
   </si>
   <si>
-    <t>2.507</t>
-  </si>
-  <si>
     <t>3.817</t>
   </si>
   <si>
@@ -390,48 +252,15 @@
     <t>2.372</t>
   </si>
   <si>
-    <t>0.008</t>
-  </si>
-  <si>
-    <t>0.045</t>
-  </si>
-  <si>
     <t>0.098</t>
   </si>
   <si>
-    <t>5.963</t>
-  </si>
-  <si>
-    <t>8.600</t>
-  </si>
-  <si>
-    <t>6.153</t>
-  </si>
-  <si>
-    <t>5.265</t>
-  </si>
-  <si>
-    <t>5.494</t>
-  </si>
-  <si>
     <t>7.116</t>
   </si>
   <si>
     <t>9.455</t>
   </si>
   <si>
-    <t>11.253</t>
-  </si>
-  <si>
-    <t>16.305</t>
-  </si>
-  <si>
-    <t>46.520</t>
-  </si>
-  <si>
-    <t>116.418</t>
-  </si>
-  <si>
     <t>0.697</t>
   </si>
   <si>
@@ -444,12 +273,6 @@
     <t>1.324</t>
   </si>
   <si>
-    <t>7.497</t>
-  </si>
-  <si>
-    <t>20.084</t>
-  </si>
-  <si>
     <t>17.049</t>
   </si>
   <si>
@@ -462,31 +285,283 @@
     <t>0.003</t>
   </si>
   <si>
-    <t>47.185</t>
-  </si>
-  <si>
-    <t>98.665</t>
-  </si>
-  <si>
-    <t>59.597</t>
-  </si>
-  <si>
-    <t>43.522</t>
-  </si>
-  <si>
     <t>47.210</t>
   </si>
   <si>
     <t>TimeGPT (few-shot)</t>
   </si>
   <si>
-    <t>4.129</t>
-  </si>
-  <si>
     <t>de_small</t>
   </si>
   <si>
     <t>de_big</t>
+  </si>
+  <si>
+    <t>0.269</t>
+  </si>
+  <si>
+    <t>1.969</t>
+  </si>
+  <si>
+    <t>0.468</t>
+  </si>
+  <si>
+    <t>1.118</t>
+  </si>
+  <si>
+    <t>0.626</t>
+  </si>
+  <si>
+    <t>1.422</t>
+  </si>
+  <si>
+    <t>0.909</t>
+  </si>
+  <si>
+    <t>1.701</t>
+  </si>
+  <si>
+    <t>1.291</t>
+  </si>
+  <si>
+    <t>1.794</t>
+  </si>
+  <si>
+    <t>1.204</t>
+  </si>
+  <si>
+    <t>1.872</t>
+  </si>
+  <si>
+    <t>2.325</t>
+  </si>
+  <si>
+    <t>2.239</t>
+  </si>
+  <si>
+    <t>3.271</t>
+  </si>
+  <si>
+    <t>2.844</t>
+  </si>
+  <si>
+    <t>4.791</t>
+  </si>
+  <si>
+    <t>4.094</t>
+  </si>
+  <si>
+    <t>6.655</t>
+  </si>
+  <si>
+    <t>0.926</t>
+  </si>
+  <si>
+    <t>2.794</t>
+  </si>
+  <si>
+    <t>0.054</t>
+  </si>
+  <si>
+    <t>0.016</t>
+  </si>
+  <si>
+    <t>0.051</t>
+  </si>
+  <si>
+    <t>0.062</t>
+  </si>
+  <si>
+    <t>0.038</t>
+  </si>
+  <si>
+    <t>0.075</t>
+  </si>
+  <si>
+    <t>0.028</t>
+  </si>
+  <si>
+    <t>0.123</t>
+  </si>
+  <si>
+    <t>0.031</t>
+  </si>
+  <si>
+    <t>0.148</t>
+  </si>
+  <si>
+    <t>1.174</t>
+  </si>
+  <si>
+    <t>4.487</t>
+  </si>
+  <si>
+    <t>1.440</t>
+  </si>
+  <si>
+    <t>2.621</t>
+  </si>
+  <si>
+    <t>1.656</t>
+  </si>
+  <si>
+    <t>2.456</t>
+  </si>
+  <si>
+    <t>3.735</t>
+  </si>
+  <si>
+    <t>3.483</t>
+  </si>
+  <si>
+    <t>3.356</t>
+  </si>
+  <si>
+    <t>5.979</t>
+  </si>
+  <si>
+    <t>1470.311</t>
+  </si>
+  <si>
+    <t>1554.456</t>
+  </si>
+  <si>
+    <t>1374.993</t>
+  </si>
+  <si>
+    <t>1771.796</t>
+  </si>
+  <si>
+    <t>762.589</t>
+  </si>
+  <si>
+    <t>878.724</t>
+  </si>
+  <si>
+    <t>2205.256</t>
+  </si>
+  <si>
+    <t>3385.276</t>
+  </si>
+  <si>
+    <t>2012.095</t>
+  </si>
+  <si>
+    <t>2323.418</t>
+  </si>
+  <si>
+    <t>2406.51</t>
+  </si>
+  <si>
+    <t>2338.977</t>
+  </si>
+  <si>
+    <t>2686.644</t>
+  </si>
+  <si>
+    <t>2614.634</t>
+  </si>
+  <si>
+    <t>0.379</t>
+  </si>
+  <si>
+    <t>0.659</t>
+  </si>
+  <si>
+    <t>1.859</t>
+  </si>
+  <si>
+    <t>3.180</t>
+  </si>
+  <si>
+    <t>1.864</t>
+  </si>
+  <si>
+    <t>4.238</t>
+  </si>
+  <si>
+    <t>7.927</t>
+  </si>
+  <si>
+    <t>8.212</t>
+  </si>
+  <si>
+    <t>16.022</t>
+  </si>
+  <si>
+    <t>13.414</t>
+  </si>
+  <si>
+    <t>36.218</t>
+  </si>
+  <si>
+    <t>26.748</t>
+  </si>
+  <si>
+    <t>67.737</t>
+  </si>
+  <si>
+    <t>1.028</t>
+  </si>
+  <si>
+    <t>17.27</t>
+  </si>
+  <si>
+    <t>0.005</t>
+  </si>
+  <si>
+    <t>0.007</t>
+  </si>
+  <si>
+    <t>0.001</t>
+  </si>
+  <si>
+    <t>0.019</t>
+  </si>
+  <si>
+    <t>0.025</t>
+  </si>
+  <si>
+    <t>1.881</t>
+  </si>
+  <si>
+    <t>24.472</t>
+  </si>
+  <si>
+    <t>25.004</t>
+  </si>
+  <si>
+    <t>2.583</t>
+  </si>
+  <si>
+    <t>11.138</t>
+  </si>
+  <si>
+    <t>22.633</t>
+  </si>
+  <si>
+    <t>3.601</t>
+  </si>
+  <si>
+    <t>9.613</t>
+  </si>
+  <si>
+    <t>22.022</t>
+  </si>
+  <si>
+    <t>32.456</t>
+  </si>
+  <si>
+    <t>22.107</t>
+  </si>
+  <si>
+    <t>112.901</t>
+  </si>
+  <si>
+    <t>23.352</t>
+  </si>
+  <si>
+    <t>102.149</t>
   </si>
 </sst>
 </file>
@@ -809,8 +884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6080771B-968D-4139-AF07-E0D46FA87262}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y30" sqref="G1:Y30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,22 +898,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>147</v>
+        <v>84</v>
       </c>
       <c r="F1" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -852,10 +927,13 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>88</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -869,10 +947,13 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>101</v>
+        <v>90</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -886,10 +967,13 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -903,10 +987,13 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>94</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -920,10 +1007,13 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -937,10 +1027,13 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>63</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -954,10 +1047,13 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -971,10 +1067,13 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>101</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -988,10 +1087,13 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1005,10 +1107,13 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>104</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>105</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1022,10 +1127,13 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E12" t="s">
-        <v>109</v>
+        <v>64</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1039,10 +1147,13 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>110</v>
+        <v>65</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1056,10 +1167,13 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>111</v>
+        <v>66</v>
+      </c>
+      <c r="F14">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1073,10 +1187,13 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>112</v>
+        <v>67</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1090,13 +1207,16 @@
         <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>24</v>
       </c>
@@ -1107,13 +1227,16 @@
         <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="F17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>96</v>
       </c>
@@ -1124,13 +1247,16 @@
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="F18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>192</v>
       </c>
@@ -1141,13 +1267,16 @@
         <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>69</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>336</v>
       </c>
@@ -1158,13 +1287,16 @@
         <v>8</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="F20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>720</v>
       </c>
@@ -1175,13 +1307,16 @@
         <v>8</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>24</v>
       </c>
@@ -1192,13 +1327,16 @@
         <v>8</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>96</v>
       </c>
@@ -1209,13 +1347,16 @@
         <v>8</v>
       </c>
       <c r="D23" t="s">
-        <v>31</v>
+        <v>110</v>
       </c>
       <c r="E23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>192</v>
       </c>
@@ -1226,13 +1367,16 @@
         <v>8</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="F24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>336</v>
       </c>
@@ -1243,13 +1387,16 @@
         <v>8</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="E25" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>720</v>
       </c>
@@ -1260,13 +1407,16 @@
         <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="E26" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>24</v>
       </c>
@@ -1277,13 +1427,16 @@
         <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="E27" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="F27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>96</v>
       </c>
@@ -1294,13 +1447,16 @@
         <v>8</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
       <c r="E28" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="F28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>192</v>
       </c>
@@ -1311,13 +1467,16 @@
         <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="E29" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>336</v>
       </c>
@@ -1328,13 +1487,16 @@
         <v>8</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>124</v>
       </c>
       <c r="E30" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>720</v>
       </c>
@@ -1345,13 +1507,16 @@
         <v>8</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="E31" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="F31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>24</v>
       </c>
@@ -1365,6 +1530,9 @@
         <v>10000</v>
       </c>
       <c r="E32">
+        <v>10000</v>
+      </c>
+      <c r="F32">
         <v>10000</v>
       </c>
     </row>
@@ -1384,6 +1552,9 @@
       <c r="E33">
         <v>10000</v>
       </c>
+      <c r="F33">
+        <v>10000</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
@@ -1401,6 +1572,9 @@
       <c r="E34">
         <v>10000</v>
       </c>
+      <c r="F34">
+        <v>10000</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
@@ -1418,16 +1592,28 @@
       <c r="E35">
         <v>10000</v>
       </c>
+      <c r="F35">
+        <v>10000</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
         <v>8</v>
+      </c>
+      <c r="D36">
+        <v>2463</v>
+      </c>
+      <c r="E36" t="s">
+        <v>128</v>
+      </c>
+      <c r="F36">
+        <v>10000</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -1435,10 +1621,19 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="C37" t="s">
         <v>8</v>
+      </c>
+      <c r="D37">
+        <v>3185</v>
+      </c>
+      <c r="E37" t="s">
+        <v>129</v>
+      </c>
+      <c r="F37">
+        <v>10000</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -1446,10 +1641,19 @@
         <v>48</v>
       </c>
       <c r="B38" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
         <v>8</v>
+      </c>
+      <c r="D38">
+        <v>5817</v>
+      </c>
+      <c r="E38" t="s">
+        <v>130</v>
+      </c>
+      <c r="F38">
+        <v>10000</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -1457,10 +1661,19 @@
         <v>60</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="C39" t="s">
         <v>8</v>
+      </c>
+      <c r="D39">
+        <v>6444</v>
+      </c>
+      <c r="E39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F39">
+        <v>10000</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -1468,10 +1681,19 @@
         <v>24</v>
       </c>
       <c r="B40" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="C40" t="s">
         <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40">
+        <v>10000</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -1479,10 +1701,19 @@
         <v>96</v>
       </c>
       <c r="B41" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
         <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>134</v>
+      </c>
+      <c r="E41" t="s">
+        <v>135</v>
+      </c>
+      <c r="F41">
+        <v>10000</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -1490,10 +1721,19 @@
         <v>192</v>
       </c>
       <c r="B42" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
         <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>136</v>
+      </c>
+      <c r="E42" t="s">
+        <v>137</v>
+      </c>
+      <c r="F42">
+        <v>10000</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -1501,10 +1741,19 @@
         <v>336</v>
       </c>
       <c r="B43" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
         <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>138</v>
+      </c>
+      <c r="E43" t="s">
+        <v>139</v>
+      </c>
+      <c r="F43">
+        <v>10000</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -1512,10 +1761,19 @@
         <v>720</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="C44" t="s">
         <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44" t="s">
+        <v>141</v>
+      </c>
+      <c r="F44">
+        <v>10000</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -1529,13 +1787,13 @@
         <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="E45" t="s">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="F45" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
@@ -1549,13 +1807,13 @@
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>36</v>
+        <v>142</v>
       </c>
       <c r="E46" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="F46" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
@@ -1569,13 +1827,13 @@
         <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>37</v>
+        <v>143</v>
       </c>
       <c r="E47" t="s">
-        <v>98</v>
+        <v>58</v>
       </c>
       <c r="F47" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -1589,13 +1847,13 @@
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="E48" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="F48" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -1609,13 +1867,13 @@
         <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>39</v>
+        <v>145</v>
       </c>
       <c r="E49" t="s">
-        <v>126</v>
+        <v>73</v>
       </c>
       <c r="F49" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1629,13 +1887,13 @@
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="E50" t="s">
-        <v>127</v>
+        <v>74</v>
       </c>
       <c r="F50" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -1649,13 +1907,13 @@
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="E51" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="F51" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -1669,13 +1927,13 @@
         <v>9</v>
       </c>
       <c r="D52" t="s">
-        <v>42</v>
+        <v>149</v>
       </c>
       <c r="E52" t="s">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="F52" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -1689,13 +1947,13 @@
         <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>43</v>
+        <v>151</v>
       </c>
       <c r="E53" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c r="F53" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -1709,13 +1967,13 @@
         <v>9</v>
       </c>
       <c r="D54" t="s">
-        <v>44</v>
+        <v>153</v>
       </c>
       <c r="E54" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="F54" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -1729,13 +1987,13 @@
         <v>9</v>
       </c>
       <c r="D55" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="E55" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="F55" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -1749,13 +2007,13 @@
         <v>9</v>
       </c>
       <c r="D56" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="E56" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="F56" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
@@ -1769,13 +2027,13 @@
         <v>9</v>
       </c>
       <c r="D57" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="E57" t="s">
-        <v>133</v>
+        <v>76</v>
       </c>
       <c r="F57" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -1789,13 +2047,13 @@
         <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="E58" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
       <c r="F58" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -1809,13 +2067,13 @@
         <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="E59" t="s">
-        <v>135</v>
+        <v>78</v>
       </c>
       <c r="F59" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -1829,13 +2087,13 @@
         <v>9</v>
       </c>
       <c r="D60" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E60" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="F60" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
@@ -1849,13 +2107,13 @@
         <v>9</v>
       </c>
       <c r="D61" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="E61" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="F61" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
@@ -1869,13 +2127,13 @@
         <v>9</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E62" t="s">
-        <v>138</v>
+        <v>79</v>
       </c>
       <c r="F62" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
@@ -1889,13 +2147,13 @@
         <v>9</v>
       </c>
       <c r="D63" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>140</v>
+        <v>81</v>
       </c>
       <c r="F63" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -1909,13 +2167,13 @@
         <v>9</v>
       </c>
       <c r="D64" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="E64" t="s">
-        <v>139</v>
+        <v>80</v>
       </c>
       <c r="F64" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
@@ -1929,13 +2187,13 @@
         <v>9</v>
       </c>
       <c r="D65" t="s">
-        <v>53</v>
+        <v>82</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
@@ -1949,13 +2207,13 @@
         <v>9</v>
       </c>
       <c r="D66" t="s">
-        <v>54</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="E66" t="s">
+        <v>157</v>
       </c>
       <c r="F66" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
@@ -1969,13 +2227,13 @@
         <v>9</v>
       </c>
       <c r="D67" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E67" t="s">
-        <v>84</v>
+        <v>158</v>
       </c>
       <c r="F67" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
@@ -1989,13 +2247,13 @@
         <v>9</v>
       </c>
       <c r="D68" t="s">
-        <v>56</v>
+        <v>159</v>
       </c>
       <c r="E68" t="s">
-        <v>141</v>
+        <v>160</v>
       </c>
       <c r="F68" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -2009,13 +2267,13 @@
         <v>9</v>
       </c>
       <c r="D69" t="s">
-        <v>56</v>
+        <v>159</v>
       </c>
       <c r="E69" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="F69" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -2029,10 +2287,13 @@
         <v>9</v>
       </c>
       <c r="D70" t="s">
-        <v>91</v>
+        <v>162</v>
       </c>
       <c r="E70" t="s">
-        <v>142</v>
+        <v>163</v>
+      </c>
+      <c r="F70" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
@@ -2046,10 +2307,13 @@
         <v>9</v>
       </c>
       <c r="D71" t="s">
-        <v>92</v>
+        <v>165</v>
       </c>
       <c r="E71" t="s">
-        <v>143</v>
+        <v>166</v>
+      </c>
+      <c r="F71" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
@@ -2063,10 +2327,13 @@
         <v>9</v>
       </c>
       <c r="D72" t="s">
-        <v>93</v>
+        <v>168</v>
       </c>
       <c r="E72" t="s">
-        <v>144</v>
+        <v>169</v>
+      </c>
+      <c r="F72" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
@@ -2080,10 +2347,13 @@
         <v>9</v>
       </c>
       <c r="D73" t="s">
-        <v>94</v>
+        <v>171</v>
       </c>
       <c r="E73" t="s">
-        <v>145</v>
+        <v>172</v>
+      </c>
+      <c r="F73" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
@@ -2097,10 +2367,13 @@
         <v>9</v>
       </c>
       <c r="D74" t="s">
-        <v>95</v>
+        <v>174</v>
       </c>
       <c r="E74" t="s">
-        <v>146</v>
+        <v>83</v>
+      </c>
+      <c r="F74" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -2188,10 +2461,19 @@
         <v>24</v>
       </c>
       <c r="B79" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="C79" t="s">
         <v>9</v>
+      </c>
+      <c r="D79">
+        <v>10000</v>
+      </c>
+      <c r="E79">
+        <v>10000</v>
+      </c>
+      <c r="F79">
+        <v>10000</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
@@ -2199,87 +2481,159 @@
         <v>36</v>
       </c>
       <c r="B80" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="C80" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D80">
+        <v>10000</v>
+      </c>
+      <c r="E80">
+        <v>10000</v>
+      </c>
+      <c r="F80">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>48</v>
       </c>
       <c r="B81" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="C81" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D81">
+        <v>10000</v>
+      </c>
+      <c r="E81">
+        <v>10000</v>
+      </c>
+      <c r="F81">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>60</v>
       </c>
       <c r="B82" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="C82" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D82">
+        <v>10000</v>
+      </c>
+      <c r="E82">
+        <v>10000</v>
+      </c>
+      <c r="F82">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>24</v>
       </c>
       <c r="B83" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="C83" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D83">
+        <v>10000</v>
+      </c>
+      <c r="E83">
+        <v>10000</v>
+      </c>
+      <c r="F83">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>96</v>
       </c>
       <c r="B84" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="C84" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D84">
+        <v>10000</v>
+      </c>
+      <c r="E84">
+        <v>10000</v>
+      </c>
+      <c r="F84">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>192</v>
       </c>
       <c r="B85" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="C85" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D85">
+        <v>10000</v>
+      </c>
+      <c r="E85">
+        <v>10000</v>
+      </c>
+      <c r="F85">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>336</v>
       </c>
       <c r="B86" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="C86" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D86">
+        <v>10000</v>
+      </c>
+      <c r="E86">
+        <v>10000</v>
+      </c>
+      <c r="F86">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>720</v>
       </c>
       <c r="B87" t="s">
-        <v>150</v>
+        <v>86</v>
       </c>
       <c r="C87" t="s">
         <v>9</v>
+      </c>
+      <c r="D87">
+        <v>10000</v>
+      </c>
+      <c r="E87">
+        <v>10000</v>
+      </c>
+      <c r="F87">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>